<commit_message>
Tests done for chamber
Now to make the chamber generator
</commit_message>
<xml_diff>
--- a/Dungeon tables.xlsx
+++ b/Dungeon tables.xlsx
@@ -1,32 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\DungeonGen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="From Hall" sheetId="1" r:id="rId1"/>
-    <sheet name="Side Passage" sheetId="2" r:id="rId2"/>
-    <sheet name="Passage Width" sheetId="3" r:id="rId3"/>
-    <sheet name="Turn" sheetId="4" r:id="rId4"/>
-    <sheet name="Stairs" sheetId="5" r:id="rId5"/>
-    <sheet name="From Door" sheetId="6" r:id="rId6"/>
-    <sheet name="Door" sheetId="7" r:id="rId7"/>
-    <sheet name="Room" sheetId="8" r:id="rId8"/>
-    <sheet name="Chamber" sheetId="9" r:id="rId9"/>
-    <sheet name="Special Room or Chamber" sheetId="10" r:id="rId10"/>
-    <sheet name="Pool" sheetId="11" r:id="rId11"/>
-    <sheet name="Cave" sheetId="12" r:id="rId12"/>
-    <sheet name="Exits" sheetId="13" r:id="rId13"/>
+    <sheet name="From Hall" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Side Passage" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Passage Width" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Turn" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Stairs" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="From Door" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Door" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Room" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Chamber" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Special Room or Chamber" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Pool" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Cave" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Exits" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="Unspecified"/>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="248">
   <si>
     <t>Roll</t>
   </si>
@@ -780,23 +776,38 @@
   </si>
   <si>
     <t>45 degrees right</t>
-  </si>
-  <si>
-    <t>(</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -811,7 +822,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -819,308 +830,76 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="52"/>
-    <col min="3" max="3" width="14.42578125"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1131,103 +910,104 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1235,22 +1015,25 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="23.140625"/>
-    <col min="3" max="3" width="40.140625"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1261,95 +1044,95 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1360,65 +1143,67 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>166</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1426,22 +1211,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="110.85546875"/>
-    <col min="3" max="3" width="50.85546875"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="110.892857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1452,50 +1240,50 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1506,48 +1294,48 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1558,47 +1346,47 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1609,41 +1397,43 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>197</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1651,20 +1441,25 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="55"/>
-    <col min="3" max="3" width="50.5703125"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1675,95 +1470,95 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1774,44 +1569,46 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>222</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1819,23 +1616,26 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="23"/>
-    <col min="3" max="3" width="51.42578125"/>
-    <col min="4" max="4" width="18.140625"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1849,108 +1649,108 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>231</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1961,51 +1761,51 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -2016,42 +1816,44 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2059,22 +1861,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="31.85546875"/>
-    <col min="3" max="3" width="14"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.984693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2085,119 +1890,121 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2205,20 +2012,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="71"/>
-    <col min="3" max="3" width="40.28515625"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.9795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2229,50 +2041,50 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2280,97 +2092,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -2378,28 +2190,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2407,20 +2221,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="24.7109375"/>
-    <col min="3" max="3" width="14"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.984693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2431,75 +2250,77 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2507,22 +2328,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="48.28515625"/>
-    <col min="3" max="3" width="98.42578125"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="98.4795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2533,129 +2357,126 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>248</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2663,22 +2484,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="52"/>
-    <col min="3" max="3" width="14.42578125"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2689,75 +2513,77 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2765,22 +2591,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="13.42578125"/>
-    <col min="3" max="3" width="19.5703125"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2791,42 +2620,44 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2834,20 +2665,25 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="13"/>
-    <col min="3" max="3" width="24.140625"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2858,108 +2694,110 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -2967,22 +2805,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="15.5703125"/>
-    <col min="3" max="3" width="25.42578125"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4132653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2993,86 +2834,88 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>